<commit_message>
to be commited xlsx
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>second attempt</t>
+  </si>
+  <si>
+    <t>sfdsfsdafa</t>
   </si>
 </sst>
 </file>
@@ -350,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -363,6 +366,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added excel test again
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>second attempt</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>sfafsfsdfsad</t>
+  </si>
+  <si>
+    <t>sfasfasdfsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sfsa</t>
   </si>
 </sst>
 </file>
@@ -356,27 +362,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>